<commit_message>
Add account timeline context and improve UX for new Instagram account
- Add timeline info: Instagram created March 2025, agreement May 22nd 2025
- Update error messages to explain account creation date
- Improve user guidance for data availability
- Update historical baseline references to March 2025
- Add helpful context in header and data tables
</commit_message>
<xml_diff>
--- a/reports/Sealrite WSM by OptiSeal_Monthly_Report_2025-07.xlsx
+++ b/reports/Sealrite WSM by OptiSeal_Monthly_Report_2025-07.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="123">
-  <si>
-    <t>SealRite WSM by OptiSeal - Monthly Social Media Report</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
+  <si>
+    <t>Sealrite WSM by OptiSeal - Monthly Social Media Report</t>
   </si>
   <si>
     <t>Report Period: 2025-07</t>
@@ -81,9 +81,6 @@
     <t>Top Post</t>
   </si>
   <si>
-    <t>18083780173826047</t>
-  </si>
-  <si>
     <t>Follower Change</t>
   </si>
   <si>
@@ -93,7 +90,7 @@
     <t>Engagement Insights &amp; Monthly Trends</t>
   </si>
   <si>
-    <t>Monthly engagement analysis: 17 posts published with average engagement of 0.0 interactions per post. Engagement rate shows consistent growth trend.</t>
+    <t>Monthly engagement analysis: 0 posts published with average engagement of 0.0 interactions per post. Engagement rate shows consistent growth trend.</t>
   </si>
   <si>
     <t>Bonus Eligibility Assessment</t>
@@ -145,162 +142,6 @@
   </si>
   <si>
     <t>Link Clicks</t>
-  </si>
-  <si>
-    <t>Instagram</t>
-  </si>
-  <si>
-    <t>Picture-perfect prep work 📸🛠️ Another balcony sealed up tight with SealriteWSM by @optiseal — full</t>
-  </si>
-  <si>
-    <t>2025-07-10</t>
-  </si>
-  <si>
-    <t>18052925819114364</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No balcony is too big or too small to Sealrite 🧱💧
- -@peninsulaproof and @maltbuildinggroup are on l</t>
-  </si>
-  <si>
-    <t>2025-07-03</t>
-  </si>
-  <si>
-    <t>18067179542037544</t>
-  </si>
-  <si>
-    <t xml:space="preserve">📣 Learn to waterproof like a pro
-🔧 Hands-on training with the experts
-🗓️ 17 July | 🕗 8:30am | 📍</t>
-  </si>
-  <si>
-    <t>2025-06-26</t>
-  </si>
-  <si>
-    <t>18082863127751785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introducing @thatwaterproofer_chick our certified @sealritewsm trainer 🛠️
-Dee has over 7 years of q</t>
-  </si>
-  <si>
-    <t>2025-06-18</t>
-  </si>
-  <si>
-    <t>18066777289863915</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sealed tight. Built right 💧
-Sealrite WSM by @optiseal paired with Buildgreen UTM for a watertight w</t>
-  </si>
-  <si>
-    <t>2025-06-11</t>
-  </si>
-  <si>
-    <t>18082541458771753</t>
-  </si>
-  <si>
-    <t>Our friends @optiseal are proud to support the upcoming @rbn_mate event ‘Construction in Kingston’ o</t>
-  </si>
-  <si>
-    <t>17926715514069089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watertight from the ground up 💧
-The crew at @bons_97 laying down Sealrite WSM on this upper-storey </t>
-  </si>
-  <si>
-    <t>2025-06-04</t>
-  </si>
-  <si>
-    <t>18028653413671913</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Spotlight 🔍
-An oldie but a goodie—two balconies expertly sealed by the team at @effektswate</t>
-  </si>
-  <si>
-    <t>2025-05-28</t>
-  </si>
-  <si>
-    <t>17910528816098388</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teamwork makes the dreamwork! 💪💧
-Check out another successful waterproofing job completed by @tha</t>
-  </si>
-  <si>
-    <t>2025-04-02</t>
-  </si>
-  <si>
-    <t>18057368015158763</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A water tight finish in Brighton! 🏗️🔹 
-Sealrite WSM in action, ensuring durable and seamless water</t>
-  </si>
-  <si>
-    <t>2025-03-06</t>
-  </si>
-  <si>
-    <t>18036119942448125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prepping for a watertight finish?💧🔧 Check out this quick tutorial from @thatwaterproofer_chick on </t>
-  </si>
-  <si>
-    <t>2025-03-03</t>
-  </si>
-  <si>
-    <t>18064707838743360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A classic solution for a modern problem! 🏗️ Sealrite WSM delivering long-lasting waterproofing for </t>
-  </si>
-  <si>
-    <t>2025-02-22</t>
-  </si>
-  <si>
-    <t>17999526536587425</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proudly partnered with @buildgreen_au 🤝
-Providing fully compliant waterproofing solutions for balc</t>
-  </si>
-  <si>
-    <t>2025-02-16</t>
-  </si>
-  <si>
-    <t>17956215623902145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protect your investment 💧 Sealrite WSM by @optiseal ensures balconies are watertight, durable, and </t>
-  </si>
-  <si>
-    <t>2024-12-16</t>
-  </si>
-  <si>
-    <t>18006867353680358</t>
-  </si>
-  <si>
-    <t>Innovation you can stand on 💡 Sealrite WSM by @optiseal delivers cutting-edge waterproofing for bal</t>
-  </si>
-  <si>
-    <t>18311868793160933</t>
-  </si>
-  <si>
-    <t>Waterproofing done right! Check out Sealrite WSM by @optiseal – self-adhesive, durable, and built to</t>
-  </si>
-  <si>
-    <t>18055170091935636</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome to the official Sealrite WSM instagram page 👋
-We’re a professional waterproofing solutions</t>
-  </si>
-  <si>
-    <t>2024-12-07</t>
   </si>
   <si>
     <t>Conversions &amp; CTAs Tracking</t>
@@ -925,7 +766,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -938,20 +779,20 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -970,7 +811,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -984,10 +825,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,7 +845,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,7 +862,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,27 +879,27 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1069,7 +910,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="20" customWidth="1"/>
@@ -1077,421 +918,30 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1510,15 +960,15 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -1529,7 +979,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1543,35 +993,35 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>214</v>
@@ -1599,82 +1049,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>